<commit_message>
Se Agregar un RefreshObject el objeto jbtnSiguiente
</commit_message>
<xml_diff>
--- a/Data/polizas.xlsx
+++ b/Data/polizas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Proyectos UFT\Acsel_AutosA004\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59D7284B-EF0E-4841-AD13-25CE01E7FE8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25DE8B5B-BB77-4AE4-9F7E-2AA8936A8A8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="19440" windowHeight="14880" activeTab="1" xr2:uid="{6115F1F8-2DE2-43A0-909F-E2FF43A424F1}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="19440" windowHeight="14880" xr2:uid="{6115F1F8-2DE2-43A0-909F-E2FF43A424F1}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="7">
   <si>
     <t>Producto</t>
   </si>
@@ -407,10 +407,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A564A74-3C94-4E5B-90A3-F5F51F21B165}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -457,6 +457,50 @@
       </c>
       <c r="C4">
         <v>1000355</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>70</v>
+      </c>
+      <c r="C5">
+        <v>1000358</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6">
+        <v>70</v>
+      </c>
+      <c r="C6">
+        <v>1000359</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7">
+        <v>70</v>
+      </c>
+      <c r="C7">
+        <v>1000360</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8">
+        <v>70</v>
+      </c>
+      <c r="C8">
+        <v>1000361</v>
       </c>
     </row>
   </sheetData>
@@ -468,7 +512,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3D6507F-4F8E-4743-948E-E73007A3DF93}">
   <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>

</xml_diff>